<commit_message>
Iniciando download da ata na versão em Excel
</commit_message>
<xml_diff>
--- a/server/sisata/src/main/resources/templates/template2.xlsx
+++ b/server/sisata/src/main/resources/templates/template2.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\repos\ProjectSisatas\server\sisata\src\main\resources\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wesley\Documents\GitHub\ProjectSisatas\server\sisata\src\main\resources\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6186628D-7464-4465-8347-3D3192106FDE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C8A6FEA-7CA4-4982-BE2D-9D5334C5F451}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ata" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">ata!$B$2:$F$22,ata!$B$27:$F$37</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">ata!$B$2:$F$21,ata!$B$26:$F$36</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <webPublishing allowPng="1" targetScreenSize="1024x768" codePage="1201"/>
@@ -64,9 +64,6 @@
   </si>
   <si>
     <t>PRAZO</t>
-  </si>
-  <si>
-    <t>DISTRIBUIÇÃO:</t>
   </si>
   <si>
     <t>Representante</t>
@@ -138,6 +135,9 @@
   </si>
   <si>
     <t>YY/YY/YYYY</t>
+  </si>
+  <si>
+    <t>DISTRIBUIÇÃO</t>
   </si>
 </sst>
 </file>
@@ -368,7 +368,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
@@ -399,12 +399,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -443,9 +437,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -454,42 +445,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
@@ -500,7 +455,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -556,6 +517,33 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -927,10 +915,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:X999"/>
+  <dimension ref="B1:X998"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27:F27"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -970,15 +958,15 @@
       <c r="X1" s="2"/>
     </row>
     <row r="2" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B2" s="45" t="s">
+      <c r="B2" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="32"/>
+      <c r="D2" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="15" t="s">
-        <v>15</v>
-      </c>
       <c r="E2" s="4"/>
-      <c r="F2" s="50"/>
+      <c r="F2" s="37"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
@@ -999,15 +987,15 @@
       <c r="X2" s="2"/>
     </row>
     <row r="3" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B3" s="46"/>
-      <c r="C3" s="47"/>
-      <c r="D3" s="16" t="s">
+      <c r="B3" s="33"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="51"/>
+      <c r="F3" s="38"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
@@ -1028,13 +1016,13 @@
       <c r="X3" s="2"/>
     </row>
     <row r="4" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B4" s="48"/>
-      <c r="C4" s="49"/>
-      <c r="D4" s="18" t="s">
-        <v>18</v>
+      <c r="B4" s="35"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="16" t="s">
+        <v>17</v>
       </c>
       <c r="E4" s="6"/>
-      <c r="F4" s="52"/>
+      <c r="F4" s="39"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
@@ -1061,7 +1049,7 @@
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
-      <c r="H5" s="14"/>
+      <c r="H5" s="12"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
@@ -1080,13 +1068,13 @@
       <c r="X5" s="2"/>
     </row>
     <row r="6" spans="2:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="32" t="s">
+      <c r="B6" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="33"/>
-      <c r="D6" s="33"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="34"/>
+      <c r="C6" s="53"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="53"/>
+      <c r="F6" s="54"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
@@ -1110,7 +1098,7 @@
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
-      <c r="E7" s="19"/>
+      <c r="E7" s="17"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
@@ -1132,13 +1120,13 @@
       <c r="X7" s="2"/>
     </row>
     <row r="8" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B8" s="35" t="s">
-        <v>19</v>
+      <c r="B8" s="55" t="s">
+        <v>18</v>
       </c>
-      <c r="C8" s="36"/>
-      <c r="D8" s="36"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="37"/>
+      <c r="C8" s="56"/>
+      <c r="D8" s="56"/>
+      <c r="E8" s="56"/>
+      <c r="F8" s="32"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
@@ -1159,10 +1147,10 @@
       <c r="X8" s="2"/>
     </row>
     <row r="9" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B9" s="59" t="s">
+      <c r="B9" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="60"/>
+      <c r="C9" s="47"/>
       <c r="D9" s="1" t="s">
         <v>2</v>
       </c>
@@ -1192,18 +1180,18 @@
       <c r="X9" s="2"/>
     </row>
     <row r="10" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B10" s="61" t="s">
+      <c r="B10" s="48" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="30"/>
+      <c r="D10" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="30"/>
-      <c r="D10" s="20" t="s">
+      <c r="E10" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="22" t="s">
+      <c r="F10" s="7" t="s">
         <v>22</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>23</v>
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
@@ -1225,18 +1213,18 @@
       <c r="X10" s="2"/>
     </row>
     <row r="11" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B11" s="62" t="s">
+      <c r="B11" s="49" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="50"/>
+      <c r="D11" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="63"/>
-      <c r="D11" s="8" t="s">
+      <c r="E11" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="F11" s="6" t="s">
         <v>26</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>27</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
@@ -1283,13 +1271,13 @@
       <c r="X12" s="2"/>
     </row>
     <row r="13" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B13" s="42" t="s">
+      <c r="B13" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="43"/>
-      <c r="D13" s="43"/>
-      <c r="E13" s="43"/>
-      <c r="F13" s="44"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="29"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
@@ -1310,18 +1298,18 @@
       <c r="X13" s="2"/>
     </row>
     <row r="14" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B14" s="53" t="s">
-        <v>28</v>
+      <c r="B14" s="40" t="s">
+        <v>27</v>
       </c>
-      <c r="C14" s="54"/>
-      <c r="D14" s="54"/>
-      <c r="E14" s="54"/>
-      <c r="F14" s="55"/>
+      <c r="C14" s="41"/>
+      <c r="D14" s="41"/>
+      <c r="E14" s="41"/>
+      <c r="F14" s="42"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
-      <c r="K14" s="29"/>
+      <c r="K14" s="26"/>
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
@@ -1346,7 +1334,7 @@
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
-      <c r="K15" s="28"/>
+      <c r="K15" s="25"/>
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
@@ -1362,18 +1350,18 @@
       <c r="X15" s="2"/>
     </row>
     <row r="16" spans="2:24" ht="59.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="56" t="s">
-        <v>29</v>
+      <c r="B16" s="43" t="s">
+        <v>28</v>
       </c>
-      <c r="C16" s="57"/>
-      <c r="D16" s="57"/>
-      <c r="E16" s="57"/>
-      <c r="F16" s="58"/>
+      <c r="C16" s="44"/>
+      <c r="D16" s="44"/>
+      <c r="E16" s="44"/>
+      <c r="F16" s="45"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
-      <c r="K16" s="28"/>
+      <c r="K16" s="25"/>
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
@@ -1398,7 +1386,7 @@
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
-      <c r="K17" s="28"/>
+      <c r="K17" s="25"/>
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
@@ -1417,11 +1405,11 @@
       <c r="B18" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="36" t="s">
+      <c r="C18" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="D18" s="36"/>
-      <c r="E18" s="23" t="s">
+      <c r="D18" s="56"/>
+      <c r="E18" s="21" t="s">
         <v>8</v>
       </c>
       <c r="F18" s="10" t="s">
@@ -1431,7 +1419,7 @@
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
-      <c r="K18" s="28"/>
+      <c r="K18" s="25"/>
       <c r="L18" s="2"/>
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
@@ -1447,24 +1435,24 @@
       <c r="X18" s="2"/>
     </row>
     <row r="19" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B19" s="21">
+      <c r="B19" s="19">
         <v>1</v>
       </c>
-      <c r="C19" s="39" t="s">
-        <v>30</v>
+      <c r="C19" s="58" t="s">
+        <v>29</v>
       </c>
-      <c r="D19" s="40"/>
-      <c r="E19" s="24" t="s">
-        <v>20</v>
+      <c r="D19" s="59"/>
+      <c r="E19" s="22" t="s">
+        <v>19</v>
       </c>
       <c r="F19" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
-      <c r="K19" s="28"/>
+      <c r="K19" s="25"/>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
@@ -1480,24 +1468,24 @@
       <c r="X19" s="2"/>
     </row>
     <row r="20" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B20" s="21">
+      <c r="B20" s="19">
         <v>2</v>
       </c>
-      <c r="C20" s="39" t="s">
+      <c r="C20" s="58" t="s">
+        <v>31</v>
+      </c>
+      <c r="D20" s="59"/>
+      <c r="E20" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="F20" s="24" t="s">
         <v>32</v>
-      </c>
-      <c r="D20" s="40"/>
-      <c r="E20" s="25" t="s">
-        <v>24</v>
-      </c>
-      <c r="F20" s="27" t="s">
-        <v>33</v>
       </c>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
-      <c r="K20" s="28"/>
+      <c r="K20" s="25"/>
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
@@ -1513,16 +1501,18 @@
       <c r="X20" s="2"/>
     </row>
     <row r="21" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B21" s="12"/>
-      <c r="C21" s="41"/>
-      <c r="D21" s="41"/>
-      <c r="E21" s="26"/>
-      <c r="F21" s="13"/>
+      <c r="B21" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" s="28"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="28"/>
+      <c r="F21" s="29"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
-      <c r="K21" s="28"/>
+      <c r="K21" s="25"/>
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
@@ -1538,18 +1528,16 @@
       <c r="X21" s="2"/>
     </row>
     <row r="22" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B22" s="42" t="s">
-        <v>10</v>
-      </c>
-      <c r="C22" s="43"/>
-      <c r="D22" s="43"/>
-      <c r="E22" s="43"/>
-      <c r="F22" s="44"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
-      <c r="K22" s="28"/>
+      <c r="K22" s="25"/>
       <c r="L22" s="2"/>
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
@@ -1574,7 +1562,7 @@
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
-      <c r="K23" s="28"/>
+      <c r="K23" s="2"/>
       <c r="L23" s="2"/>
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
@@ -1640,11 +1628,13 @@
       <c r="X25" s="2"/>
     </row>
     <row r="26" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
+      <c r="B26" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" s="30"/>
+      <c r="D26" s="30"/>
+      <c r="E26" s="30"/>
+      <c r="F26" s="30"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
@@ -1665,7 +1655,7 @@
       <c r="X26" s="2"/>
     </row>
     <row r="27" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B27" s="30" t="s">
+      <c r="B27" s="51" t="s">
         <v>11</v>
       </c>
       <c r="C27" s="30"/>
@@ -1692,7 +1682,7 @@
       <c r="X27" s="2"/>
     </row>
     <row r="28" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B28" s="31" t="s">
+      <c r="B28" s="30" t="s">
         <v>12</v>
       </c>
       <c r="C28" s="30"/>
@@ -1719,13 +1709,11 @@
       <c r="X28" s="2"/>
     </row>
     <row r="29" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B29" s="30" t="s">
-        <v>13</v>
-      </c>
-      <c r="C29" s="30"/>
-      <c r="D29" s="30"/>
-      <c r="E29" s="30"/>
-      <c r="F29" s="30"/>
+      <c r="B29" s="57"/>
+      <c r="C29" s="57"/>
+      <c r="D29" s="57"/>
+      <c r="E29" s="57"/>
+      <c r="F29" s="57"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
@@ -1746,11 +1734,13 @@
       <c r="X29" s="2"/>
     </row>
     <row r="30" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B30" s="38"/>
-      <c r="C30" s="38"/>
-      <c r="D30" s="38"/>
-      <c r="E30" s="38"/>
-      <c r="F30" s="38"/>
+      <c r="B30" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="C30" s="30"/>
+      <c r="D30" s="30"/>
+      <c r="E30" s="30"/>
+      <c r="F30" s="30"/>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
@@ -1825,13 +1815,11 @@
       <c r="X32" s="2"/>
     </row>
     <row r="33" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B33" s="30" t="s">
-        <v>13</v>
-      </c>
-      <c r="C33" s="30"/>
-      <c r="D33" s="30"/>
-      <c r="E33" s="30"/>
-      <c r="F33" s="30"/>
+      <c r="B33" s="57"/>
+      <c r="C33" s="57"/>
+      <c r="D33" s="57"/>
+      <c r="E33" s="57"/>
+      <c r="F33" s="57"/>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
@@ -1852,11 +1840,13 @@
       <c r="X33" s="2"/>
     </row>
     <row r="34" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B34" s="38"/>
-      <c r="C34" s="38"/>
-      <c r="D34" s="38"/>
-      <c r="E34" s="38"/>
-      <c r="F34" s="38"/>
+      <c r="B34" s="51" t="s">
+        <v>10</v>
+      </c>
+      <c r="C34" s="30"/>
+      <c r="D34" s="30"/>
+      <c r="E34" s="30"/>
+      <c r="F34" s="30"/>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
@@ -1877,7 +1867,7 @@
       <c r="X34" s="2"/>
     </row>
     <row r="35" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B35" s="31" t="s">
+      <c r="B35" s="30" t="s">
         <v>11</v>
       </c>
       <c r="C35" s="30"/>
@@ -1904,7 +1894,7 @@
       <c r="X35" s="2"/>
     </row>
     <row r="36" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B36" s="30" t="s">
+      <c r="B36" s="51" t="s">
         <v>12</v>
       </c>
       <c r="C36" s="30"/>
@@ -1931,13 +1921,11 @@
       <c r="X36" s="2"/>
     </row>
     <row r="37" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B37" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="C37" s="30"/>
-      <c r="D37" s="30"/>
-      <c r="E37" s="30"/>
-      <c r="F37" s="30"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
@@ -25982,35 +25970,25 @@
       <c r="W998" s="2"/>
       <c r="X998" s="2"/>
     </row>
-    <row r="999" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B999" s="2"/>
-      <c r="C999" s="2"/>
-      <c r="D999" s="2"/>
-      <c r="E999" s="2"/>
-      <c r="F999" s="2"/>
-      <c r="G999" s="2"/>
-      <c r="H999" s="2"/>
-      <c r="I999" s="2"/>
-      <c r="J999" s="2"/>
-      <c r="K999" s="2"/>
-      <c r="L999" s="2"/>
-      <c r="M999" s="2"/>
-      <c r="N999" s="2"/>
-      <c r="O999" s="2"/>
-      <c r="P999" s="2"/>
-      <c r="Q999" s="2"/>
-      <c r="R999" s="2"/>
-      <c r="S999" s="2"/>
-      <c r="T999" s="2"/>
-      <c r="U999" s="2"/>
-      <c r="V999" s="2"/>
-      <c r="W999" s="2"/>
-      <c r="X999" s="2"/>
-    </row>
   </sheetData>
-  <mergeCells count="26">
-    <mergeCell ref="B22:F22"/>
+  <mergeCells count="25">
+    <mergeCell ref="B35:F35"/>
+    <mergeCell ref="B36:F36"/>
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="B29:F29"/>
+    <mergeCell ref="B33:F33"/>
     <mergeCell ref="B27:F27"/>
+    <mergeCell ref="B28:F28"/>
+    <mergeCell ref="B30:F30"/>
+    <mergeCell ref="B31:F31"/>
+    <mergeCell ref="B32:F32"/>
+    <mergeCell ref="B34:F34"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="B26:F26"/>
     <mergeCell ref="B2:C4"/>
     <mergeCell ref="F2:F4"/>
     <mergeCell ref="B13:F13"/>
@@ -26019,22 +25997,6 @@
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B36:F36"/>
-    <mergeCell ref="B37:F37"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="B30:F30"/>
-    <mergeCell ref="B34:F34"/>
-    <mergeCell ref="B28:F28"/>
-    <mergeCell ref="B29:F29"/>
-    <mergeCell ref="B31:F31"/>
-    <mergeCell ref="B32:F32"/>
-    <mergeCell ref="B33:F33"/>
-    <mergeCell ref="B35:F35"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="5" orientation="portrait" r:id="rId1"/>
@@ -26046,15 +26008,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DF3CEA3A9869A24E908C80E629A011B0" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="daaeb6e23fe035e53945bf52281eec93">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="4cdb0f69-8f23-4e34-9e7e-d984a4ab66dc" xmlns:ns4="6cc8bd0d-fc35-46fb-9f3e-98771e35dc48" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c667dd57fcfae6b236bbf1687db50bc1" ns3:_="" ns4:_="">
     <xsd:import namespace="4cdb0f69-8f23-4e34-9e7e-d984a4ab66dc"/>
@@ -26251,6 +26204,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -26258,14 +26220,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5EA9B980-7D23-417C-9DD8-F61F644C7C90}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0242DE9F-656C-4C16-9824-C8E5A8871962}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -26280,6 +26234,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5EA9B980-7D23-417C-9DD8-F61F644C7C90}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Adição da observação na ata Excel
</commit_message>
<xml_diff>
--- a/server/sisata/src/main/resources/templates/template2.xlsx
+++ b/server/sisata/src/main/resources/templates/template2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wesley\Documents\GitHub\ProjectSisatas\server\sisata\src\main\resources\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C8A6FEA-7CA4-4982-BE2D-9D5334C5F451}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B4AD334-1997-46A5-B068-0F352D9B3770}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -446,6 +446,39 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -455,13 +488,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -517,33 +544,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -917,8 +917,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:X998"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -958,15 +958,15 @@
       <c r="X1" s="2"/>
     </row>
     <row r="2" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="32"/>
+      <c r="C2" s="34"/>
       <c r="D2" s="13" t="s">
         <v>14</v>
       </c>
       <c r="E2" s="4"/>
-      <c r="F2" s="37"/>
+      <c r="F2" s="46"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
@@ -987,15 +987,15 @@
       <c r="X2" s="2"/>
     </row>
     <row r="3" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B3" s="33"/>
-      <c r="C3" s="34"/>
+      <c r="B3" s="42"/>
+      <c r="C3" s="43"/>
       <c r="D3" s="14" t="s">
         <v>15</v>
       </c>
       <c r="E3" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="38"/>
+      <c r="F3" s="47"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
@@ -1016,13 +1016,13 @@
       <c r="X3" s="2"/>
     </row>
     <row r="4" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B4" s="35"/>
-      <c r="C4" s="36"/>
+      <c r="B4" s="44"/>
+      <c r="C4" s="45"/>
       <c r="D4" s="16" t="s">
         <v>17</v>
       </c>
       <c r="E4" s="6"/>
-      <c r="F4" s="39"/>
+      <c r="F4" s="48"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
@@ -1068,13 +1068,13 @@
       <c r="X5" s="2"/>
     </row>
     <row r="6" spans="2:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="52" t="s">
+      <c r="B6" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="53"/>
-      <c r="D6" s="53"/>
-      <c r="E6" s="53"/>
-      <c r="F6" s="54"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="31"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
@@ -1120,13 +1120,13 @@
       <c r="X7" s="2"/>
     </row>
     <row r="8" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B8" s="55" t="s">
+      <c r="B8" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="56"/>
-      <c r="D8" s="56"/>
-      <c r="E8" s="56"/>
-      <c r="F8" s="32"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="34"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
@@ -1147,10 +1147,10 @@
       <c r="X8" s="2"/>
     </row>
     <row r="9" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B9" s="46" t="s">
+      <c r="B9" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="47"/>
+      <c r="C9" s="56"/>
       <c r="D9" s="1" t="s">
         <v>2</v>
       </c>
@@ -1180,10 +1180,10 @@
       <c r="X9" s="2"/>
     </row>
     <row r="10" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B10" s="48" t="s">
+      <c r="B10" s="57" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="30"/>
+      <c r="C10" s="27"/>
       <c r="D10" s="18" t="s">
         <v>20</v>
       </c>
@@ -1213,10 +1213,10 @@
       <c r="X10" s="2"/>
     </row>
     <row r="11" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B11" s="49" t="s">
+      <c r="B11" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="50"/>
+      <c r="C11" s="59"/>
       <c r="D11" s="8" t="s">
         <v>24</v>
       </c>
@@ -1271,13 +1271,13 @@
       <c r="X12" s="2"/>
     </row>
     <row r="13" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B13" s="27" t="s">
+      <c r="B13" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="28"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="29"/>
+      <c r="C13" s="39"/>
+      <c r="D13" s="39"/>
+      <c r="E13" s="39"/>
+      <c r="F13" s="40"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
@@ -1298,13 +1298,13 @@
       <c r="X13" s="2"/>
     </row>
     <row r="14" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B14" s="40" t="s">
+      <c r="B14" s="49" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="41"/>
-      <c r="D14" s="41"/>
-      <c r="E14" s="41"/>
-      <c r="F14" s="42"/>
+      <c r="C14" s="50"/>
+      <c r="D14" s="50"/>
+      <c r="E14" s="50"/>
+      <c r="F14" s="51"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
@@ -1350,13 +1350,13 @@
       <c r="X15" s="2"/>
     </row>
     <row r="16" spans="2:24" ht="59.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="43" t="s">
+      <c r="B16" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="44"/>
-      <c r="D16" s="44"/>
-      <c r="E16" s="44"/>
-      <c r="F16" s="45"/>
+      <c r="C16" s="53"/>
+      <c r="D16" s="53"/>
+      <c r="E16" s="53"/>
+      <c r="F16" s="54"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
@@ -1405,10 +1405,10 @@
       <c r="B18" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="56" t="s">
+      <c r="C18" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="D18" s="56"/>
+      <c r="D18" s="33"/>
       <c r="E18" s="21" t="s">
         <v>8</v>
       </c>
@@ -1438,10 +1438,10 @@
       <c r="B19" s="19">
         <v>1</v>
       </c>
-      <c r="C19" s="58" t="s">
+      <c r="C19" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="D19" s="59"/>
+      <c r="D19" s="37"/>
       <c r="E19" s="22" t="s">
         <v>19</v>
       </c>
@@ -1471,10 +1471,10 @@
       <c r="B20" s="19">
         <v>2</v>
       </c>
-      <c r="C20" s="58" t="s">
+      <c r="C20" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="D20" s="59"/>
+      <c r="D20" s="37"/>
       <c r="E20" s="23" t="s">
         <v>23</v>
       </c>
@@ -1501,13 +1501,13 @@
       <c r="X20" s="2"/>
     </row>
     <row r="21" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B21" s="27" t="s">
+      <c r="B21" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="C21" s="28"/>
-      <c r="D21" s="28"/>
-      <c r="E21" s="28"/>
-      <c r="F21" s="29"/>
+      <c r="C21" s="39"/>
+      <c r="D21" s="39"/>
+      <c r="E21" s="39"/>
+      <c r="F21" s="40"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
@@ -1628,13 +1628,13 @@
       <c r="X25" s="2"/>
     </row>
     <row r="26" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B26" s="30" t="s">
+      <c r="B26" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="C26" s="30"/>
-      <c r="D26" s="30"/>
-      <c r="E26" s="30"/>
-      <c r="F26" s="30"/>
+      <c r="C26" s="27"/>
+      <c r="D26" s="27"/>
+      <c r="E26" s="27"/>
+      <c r="F26" s="27"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
@@ -1655,13 +1655,13 @@
       <c r="X26" s="2"/>
     </row>
     <row r="27" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B27" s="51" t="s">
+      <c r="B27" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="C27" s="30"/>
-      <c r="D27" s="30"/>
-      <c r="E27" s="30"/>
-      <c r="F27" s="30"/>
+      <c r="C27" s="27"/>
+      <c r="D27" s="27"/>
+      <c r="E27" s="27"/>
+      <c r="F27" s="27"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
@@ -1682,13 +1682,13 @@
       <c r="X27" s="2"/>
     </row>
     <row r="28" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B28" s="30" t="s">
+      <c r="B28" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="C28" s="30"/>
-      <c r="D28" s="30"/>
-      <c r="E28" s="30"/>
-      <c r="F28" s="30"/>
+      <c r="C28" s="27"/>
+      <c r="D28" s="27"/>
+      <c r="E28" s="27"/>
+      <c r="F28" s="27"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
@@ -1709,11 +1709,11 @@
       <c r="X28" s="2"/>
     </row>
     <row r="29" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B29" s="57"/>
-      <c r="C29" s="57"/>
-      <c r="D29" s="57"/>
-      <c r="E29" s="57"/>
-      <c r="F29" s="57"/>
+      <c r="B29" s="35"/>
+      <c r="C29" s="35"/>
+      <c r="D29" s="35"/>
+      <c r="E29" s="35"/>
+      <c r="F29" s="35"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
@@ -1734,13 +1734,13 @@
       <c r="X29" s="2"/>
     </row>
     <row r="30" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B30" s="30" t="s">
+      <c r="B30" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="C30" s="30"/>
-      <c r="D30" s="30"/>
-      <c r="E30" s="30"/>
-      <c r="F30" s="30"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
@@ -1761,13 +1761,13 @@
       <c r="X30" s="2"/>
     </row>
     <row r="31" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B31" s="30" t="s">
+      <c r="B31" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="C31" s="30"/>
-      <c r="D31" s="30"/>
-      <c r="E31" s="30"/>
-      <c r="F31" s="30"/>
+      <c r="C31" s="27"/>
+      <c r="D31" s="27"/>
+      <c r="E31" s="27"/>
+      <c r="F31" s="27"/>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
@@ -1788,13 +1788,13 @@
       <c r="X31" s="2"/>
     </row>
     <row r="32" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B32" s="30" t="s">
+      <c r="B32" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="C32" s="30"/>
-      <c r="D32" s="30"/>
-      <c r="E32" s="30"/>
-      <c r="F32" s="30"/>
+      <c r="C32" s="27"/>
+      <c r="D32" s="27"/>
+      <c r="E32" s="27"/>
+      <c r="F32" s="27"/>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
@@ -1815,11 +1815,11 @@
       <c r="X32" s="2"/>
     </row>
     <row r="33" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B33" s="57"/>
-      <c r="C33" s="57"/>
-      <c r="D33" s="57"/>
-      <c r="E33" s="57"/>
-      <c r="F33" s="57"/>
+      <c r="B33" s="35"/>
+      <c r="C33" s="35"/>
+      <c r="D33" s="35"/>
+      <c r="E33" s="35"/>
+      <c r="F33" s="35"/>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
@@ -1840,13 +1840,13 @@
       <c r="X33" s="2"/>
     </row>
     <row r="34" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B34" s="51" t="s">
+      <c r="B34" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="C34" s="30"/>
-      <c r="D34" s="30"/>
-      <c r="E34" s="30"/>
-      <c r="F34" s="30"/>
+      <c r="C34" s="27"/>
+      <c r="D34" s="27"/>
+      <c r="E34" s="27"/>
+      <c r="F34" s="27"/>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
@@ -1867,13 +1867,13 @@
       <c r="X34" s="2"/>
     </row>
     <row r="35" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B35" s="30" t="s">
+      <c r="B35" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="C35" s="30"/>
-      <c r="D35" s="30"/>
-      <c r="E35" s="30"/>
-      <c r="F35" s="30"/>
+      <c r="C35" s="27"/>
+      <c r="D35" s="27"/>
+      <c r="E35" s="27"/>
+      <c r="F35" s="27"/>
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
@@ -1894,13 +1894,13 @@
       <c r="X35" s="2"/>
     </row>
     <row r="36" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B36" s="51" t="s">
+      <c r="B36" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="C36" s="30"/>
-      <c r="D36" s="30"/>
-      <c r="E36" s="30"/>
-      <c r="F36" s="30"/>
+      <c r="C36" s="27"/>
+      <c r="D36" s="27"/>
+      <c r="E36" s="27"/>
+      <c r="F36" s="27"/>
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
       <c r="I36" s="2"/>
@@ -25972,6 +25972,15 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="B26:F26"/>
+    <mergeCell ref="B2:C4"/>
+    <mergeCell ref="F2:F4"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="B14:F14"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
     <mergeCell ref="B35:F35"/>
     <mergeCell ref="B36:F36"/>
     <mergeCell ref="B6:F6"/>
@@ -25988,15 +25997,6 @@
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="C20:D20"/>
     <mergeCell ref="B21:F21"/>
-    <mergeCell ref="B26:F26"/>
-    <mergeCell ref="B2:C4"/>
-    <mergeCell ref="F2:F4"/>
-    <mergeCell ref="B13:F13"/>
-    <mergeCell ref="B14:F14"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="5" orientation="portrait" r:id="rId1"/>
@@ -26008,6 +26008,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DF3CEA3A9869A24E908C80E629A011B0" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="daaeb6e23fe035e53945bf52281eec93">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="4cdb0f69-8f23-4e34-9e7e-d984a4ab66dc" xmlns:ns4="6cc8bd0d-fc35-46fb-9f3e-98771e35dc48" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c667dd57fcfae6b236bbf1687db50bc1" ns3:_="" ns4:_="">
     <xsd:import namespace="4cdb0f69-8f23-4e34-9e7e-d984a4ab66dc"/>
@@ -26204,15 +26213,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -26220,6 +26220,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5EA9B980-7D23-417C-9DD8-F61F644C7C90}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0242DE9F-656C-4C16-9824-C8E5A8871962}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -26234,14 +26242,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5EA9B980-7D23-417C-9DD8-F61F644C7C90}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>